<commit_message>
second excel chnages commited
</commit_message>
<xml_diff>
--- a/myexcel.xlsx
+++ b/myexcel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SCF Projects\Second-Repo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9FAC324-5D83-449F-9A5C-067C5F6AABBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68449431-4E06-46FC-B9E9-5BB74260CD4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="696" yWindow="696" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t xml:space="preserve">sr no </t>
   </si>
@@ -34,6 +34,9 @@
   </si>
   <si>
     <t>date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DashBoard </t>
   </si>
 </sst>
 </file>
@@ -69,8 +72,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -351,13 +355,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:C2"/>
+  <dimension ref="A2:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="9.6640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
@@ -368,6 +375,17 @@
       </c>
       <c r="C2" t="s">
         <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="1">
+        <v>45008</v>
       </c>
     </row>
   </sheetData>

</xml_diff>